<commit_message>
! updated velocity + added the project summary section to the report
</commit_message>
<xml_diff>
--- a/docs/supplier/VelocityChart.xlsx
+++ b/docs/supplier/VelocityChart.xlsx
@@ -148,18 +148,17 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="76813440"/>
-        <c:axId val="68917888"/>
+        <c:axId val="82271232"/>
+        <c:axId val="85599360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76813440"/>
+        <c:axId val="82271232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -185,14 +184,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68917888"/>
+        <c:crossAx val="85599360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68917888"/>
+        <c:axId val="85599360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -218,7 +217,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76813440"/>
+        <c:crossAx val="82271232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -227,7 +226,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -556,7 +555,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -593,12 +592,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <f>(20+4)/2</f>
-        <v>12</v>
+        <f>1+3+5</f>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>